<commit_message>
new test suite, removed core metrics by site logic, added set_filter method to real user report test case
</commit_message>
<xml_diff>
--- a/Data Files/Report types.xlsx
+++ b/Data Files/Report types.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bluetriangletech-my.sharepoint.com/personal/giavanna_esposito_bluetriangle_com/Documents/Documents/Test Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GiaEsposito\git\BTT_Katalon_Portal_Automation_reports\Data Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="56" documentId="8_{107678F4-7078-4827-9CF5-1BC3218D64E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4AFDE9D4-3FE7-44B3-A83A-0779969D316B}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4E457C2-0717-4E68-89A9-3A80AB595F9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{2047CC32-6F6B-4C7C-A33C-71583C7553A1}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="44">
   <si>
     <t>bounceRate</t>
   </si>
@@ -243,10 +243,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -546,10 +542,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3C4353B-294D-48CB-8020-EE8488F4FDAA}">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21:XFD21"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -759,6 +755,14 @@
         <v>43</v>
       </c>
     </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>